<commit_message>
Updated tests and docs
</commit_message>
<xml_diff>
--- a/docs/testoutputs/test_all_criteria.xlsx
+++ b/docs/testoutputs/test_all_criteria.xlsx
@@ -9,29 +9,29 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
     <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 2, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="58">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
   <si>
     <t>JobNo</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -44,27 +44,27 @@
     <t>3</t>
   </si>
   <si>
+    <t>20220325</t>
+  </si>
+  <si>
+    <t>Criteria Failing, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 2, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>/c/e</t>
   </si>
   <si>
-    <t>20220316</t>
-  </si>
-  <si>
-    <t>Criteria Failing, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 3, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 2, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -176,25 +176,22 @@
     <t>1 &amp; 2</t>
   </si>
   <si>
+    <t>Criterion 2 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 2 Relative Change (%)</t>
+  </si>
+  <si>
+    <t>Criterion 3 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 3 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 1 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 1 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
-    <t>Criterion 3 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 3 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 2 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 2 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -378,10 +375,10 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="2" name="Date"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="Author"/>
+    <tableColumn id="5" name="JobNo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -408,8 +405,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,8 +435,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 2 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 2 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,7 +770,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -787,10 +784,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -804,10 +801,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -821,7 +818,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -1265,16 +1262,16 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2.45</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>-0.04999999999999982</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>-1.999999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1285,16 +1282,16 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>7.79</v>
+        <v>14</v>
       </c>
       <c r="E3">
-        <v>-0.009999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>-0.1282051282051255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1305,16 +1302,16 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>8.09</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>-0.009999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>-0.1234567901234542</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1393,16 +1390,16 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>10.59</v>
+        <v>25</v>
       </c>
       <c r="E9">
-        <v>-0.009999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>-0.09433962264150743</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1413,16 +1410,16 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>26.04</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>0.03999999999999915</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.1538461538461506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1433,16 +1430,16 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>11.57</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>-0.02999999999999936</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.2586206896551669</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1453,16 +1450,16 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>26.34</v>
+        <v>29</v>
       </c>
       <c r="E12">
-        <v>0.03999999999999915</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.1520912547528485</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1490,10 +1487,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1510,16 +1507,16 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>0.14</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>0.04000000000000001</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>40.00000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1547,16 +1544,16 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>12.91</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>0.009999999999999787</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.07751937984495957</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1567,16 +1564,16 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>28.31</v>
+        <v>30</v>
       </c>
       <c r="E18">
-        <v>0.00999999999999801</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0.03533568904592936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1587,16 +1584,16 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>33</v>
       </c>
       <c r="D19">
-        <v>13.43</v>
+        <v>33</v>
       </c>
       <c r="E19">
-        <v>0.02999999999999936</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.2238805970149206</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1607,16 +1604,16 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>28.61</v>
+        <v>30</v>
       </c>
       <c r="E20">
-        <v>0.00999999999999801</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.03496503496502801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1627,16 +1624,16 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0.03</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1647,16 +1644,16 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>1.58</v>
+        <v>7</v>
       </c>
       <c r="E22">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>-1.250000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1667,16 +1664,16 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>0.35</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>-0.05000000000000004</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>-12.50000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1687,16 +1684,16 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0.03</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1707,16 +1704,16 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>18</v>
       </c>
       <c r="D25">
-        <v>5.58</v>
+        <v>18</v>
       </c>
       <c r="E25">
-        <v>-0.01999999999999957</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>-0.3571428571428495</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1727,16 +1724,16 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>17.75</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>0.05000000000000071</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.2824858757062187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1747,16 +1744,16 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>5.23</v>
+        <v>21</v>
       </c>
       <c r="E27">
-        <v>0.03000000000000025</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0.5769230769230818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1767,16 +1764,16 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>22</v>
       </c>
       <c r="D28">
-        <v>17.75</v>
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>0.05000000000000071</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0.2824858757062187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1882,10 +1879,10 @@
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2513,10 +2510,10 @@
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2527,10 +2524,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2547,10 +2544,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>7.8</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2567,10 +2564,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>8.1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2655,10 +2652,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2675,10 +2672,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2695,10 +2692,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2715,10 +2712,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>26.3</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2752,10 +2749,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2772,10 +2769,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2809,10 +2806,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>29</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2829,10 +2826,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2849,10 +2846,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>33</v>
+        <v>13.4</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2869,10 +2866,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2889,15 +2886,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2909,10 +2903,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2929,10 +2923,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2949,15 +2943,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2969,10 +2960,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2989,10 +2980,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -3009,10 +3000,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>21</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3029,10 +3020,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>22</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>

<commit_message>
Added li_columns_sorted so that the order of columns for TM52 and TM59 are enforced in the final report
</commit_message>
<xml_diff>
--- a/docs/testoutputs/test_all_criteria.xlsx
+++ b/docs/testoutputs/test_all_criteria.xlsx
@@ -10,8 +10,8 @@
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Criteria Failing, Air Speed 0.1" sheetId="2" r:id="rId2"/>
     <sheet name="Criterion 2, Air Speed 0.1" sheetId="3" r:id="rId3"/>
-    <sheet name="Criterion 3, Air Speed 0.1" sheetId="4" r:id="rId4"/>
-    <sheet name="Criterion 1, Air Speed 0.1" sheetId="5" r:id="rId5"/>
+    <sheet name="Criterion 1, Air Speed 0.1" sheetId="4" r:id="rId4"/>
+    <sheet name="Criterion 3, Air Speed 0.1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -20,18 +20,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="58">
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>JobNo</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -44,27 +44,27 @@
     <t>3</t>
   </si>
   <si>
+    <t>Criteria Failing, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 2, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 1, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Criterion 3, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>/c/e</t>
+  </si>
+  <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>20220325</t>
   </si>
   <si>
-    <t>Criteria Failing, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 2, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 3, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Criterion 1, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
-    <t>/c/e</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -182,16 +182,16 @@
     <t>Criterion 2 Relative Change (%)</t>
   </si>
   <si>
+    <t>Criterion 1 Absolute Change</t>
+  </si>
+  <si>
+    <t>Criterion 1 Relative Change (%)</t>
+  </si>
+  <si>
     <t>Criterion 3 Absolute Change</t>
   </si>
   <si>
     <t>Criterion 3 Relative Change (%)</t>
-  </si>
-  <si>
-    <t>Criterion 1 Absolute Change</t>
-  </si>
-  <si>
-    <t>Criterion 1 Relative Change (%)</t>
   </si>
 </sst>
 </file>
@@ -375,10 +375,10 @@
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="2" name="sheet_name"/>
+    <tableColumn id="3" name="JobNo"/>
     <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="JobNo"/>
+    <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -420,8 +420,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,8 +435,8 @@
     <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="IES Results"/>
     <tableColumn id="4" name="MF Results"/>
-    <tableColumn id="5" name="Criterion 1 Absolute Change"/>
-    <tableColumn id="6" name="Criterion 1 Relative Change (%)"/>
+    <tableColumn id="5" name="Criterion 3 Absolute Change"/>
+    <tableColumn id="6" name="Criterion 3 Relative Change (%)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -781,10 +781,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -798,10 +798,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -815,7 +815,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -1893,10 +1893,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1913,10 +1913,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1933,10 +1933,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>8.1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2021,10 +2021,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>10.6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2041,10 +2041,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2061,10 +2061,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>11.6</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2081,10 +2081,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>26.3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>26.3</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2118,10 +2118,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2138,10 +2138,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2175,10 +2175,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>12.9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2195,10 +2195,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>28.3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2215,10 +2215,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>13.4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>13.4</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2235,10 +2235,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>28.6</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>28.6</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2255,15 +2255,12 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2275,10 +2272,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2295,10 +2292,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2315,15 +2312,12 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2335,10 +2329,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>5.6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2355,10 +2349,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2375,10 +2369,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -2395,10 +2389,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>17.7</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2524,10 +2518,10 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2544,10 +2538,10 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7.8</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2564,10 +2558,10 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>8.1</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2652,10 +2646,10 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>10.6</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2672,10 +2666,10 @@
         <v>28</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2692,10 +2686,10 @@
         <v>29</v>
       </c>
       <c r="C11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2712,10 +2706,10 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>26.3</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2749,10 +2743,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2769,10 +2763,10 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2806,10 +2800,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2826,10 +2820,10 @@
         <v>36</v>
       </c>
       <c r="C18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>28.3</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2846,10 +2840,10 @@
         <v>37</v>
       </c>
       <c r="C19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>13.4</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2866,10 +2860,10 @@
         <v>38</v>
       </c>
       <c r="C20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>28.6</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2886,12 +2880,15 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
@@ -2903,10 +2900,10 @@
         <v>40</v>
       </c>
       <c r="C22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2923,10 +2920,10 @@
         <v>41</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2943,12 +2940,15 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
@@ -2960,10 +2960,10 @@
         <v>43</v>
       </c>
       <c r="C25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5.6</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2980,10 +2980,10 @@
         <v>44</v>
       </c>
       <c r="C26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -3000,10 +3000,10 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3020,10 +3020,10 @@
         <v>46</v>
       </c>
       <c r="C28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>17.7</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>0</v>

</xml_diff>